<commit_message>
Tabelle vergroessert und neue Stunden eingetragen
</commit_message>
<xml_diff>
--- a/ILV.xlsx
+++ b/ILV.xlsx
@@ -1,28 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\i00202920\Documents\GitHub\Pro1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/frank/Pro1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{2561E49C-022C-4629-B00B-5FD1B1435A9A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C97D55AA-A223-1F4E-8632-0D4B3789ACAE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="460" windowWidth="22420" windowHeight="14620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="22420" windowHeight="14620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Recherche-Dokument" sheetId="1" r:id="rId1"/>
     <sheet name="Pflichtenheft org." sheetId="2" r:id="rId2"/>
     <sheet name="Pflichtenheft techn." sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="42">
   <si>
     <t>ILV</t>
   </si>
@@ -163,6 +163,15 @@
   </si>
   <si>
     <t>Total:</t>
+  </si>
+  <si>
+    <t>Woche 4</t>
+  </si>
+  <si>
+    <t>Woche 5</t>
+  </si>
+  <si>
+    <t>Projektstrukturplan Zeiten eingetragen &amp; addiert, wo möglich</t>
   </si>
 </sst>
 </file>
@@ -710,57 +719,57 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -844,7 +853,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1140,45 +1149,58 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:F16"/>
+  <dimension ref="B2:J16"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.453125"/>
-    <col min="2" max="2" width="13.453125"/>
-    <col min="3" max="3" width="12.1796875"/>
-    <col min="4" max="4" width="39.81640625"/>
-    <col min="5" max="5" width="10.36328125"/>
-    <col min="6" max="6" width="40.36328125"/>
-    <col min="7" max="256" width="9.453125"/>
-    <col min="257" max="1025" width="11.453125"/>
+    <col min="1" max="1" width="9.5"/>
+    <col min="2" max="2" width="13.5"/>
+    <col min="3" max="3" width="12.1640625"/>
+    <col min="4" max="4" width="38.6640625" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125"/>
+    <col min="6" max="6" width="38.6640625" customWidth="1"/>
+    <col min="7" max="7" width="9.5"/>
+    <col min="8" max="8" width="38.6640625" customWidth="1"/>
+    <col min="9" max="9" width="9.5"/>
+    <col min="10" max="10" width="28.5" customWidth="1"/>
+    <col min="11" max="256" width="9.5"/>
+    <col min="257" max="1025" width="11.5"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="2:10" ht="24" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:10" ht="19" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="C7" s="30" t="s">
+    <row r="6" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="2:10" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="C7" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="30"/>
-      <c r="E7" s="32" t="s">
+      <c r="D7" s="40"/>
+      <c r="E7" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="F7" s="33"/>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="F7" s="42"/>
+      <c r="G7" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="H7" s="42"/>
+      <c r="I7" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="J7" s="42"/>
+    </row>
+    <row r="8" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C8" s="3" t="s">
         <v>4</v>
       </c>
@@ -1191,8 +1213,20 @@
       <c r="F8" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="2:6" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="G8" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" ht="97" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
         <v>6</v>
       </c>
@@ -1208,8 +1242,12 @@
       <c r="F9" s="10" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="2:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="G9" s="9"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="10"/>
+    </row>
+    <row r="10" spans="2:10" ht="48" x14ac:dyDescent="0.2">
       <c r="B10" s="11" t="s">
         <v>9</v>
       </c>
@@ -1225,8 +1263,12 @@
       <c r="F10" s="15" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="11" spans="2:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="G10" s="14"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="15"/>
+    </row>
+    <row r="11" spans="2:10" ht="48" x14ac:dyDescent="0.2">
       <c r="B11" s="11" t="s">
         <v>10</v>
       </c>
@@ -1242,8 +1284,16 @@
       <c r="F11" s="15" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" spans="2:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="G11" s="14">
+        <v>0.2</v>
+      </c>
+      <c r="H11" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="I11" s="14"/>
+      <c r="J11" s="15"/>
+    </row>
+    <row r="12" spans="2:10" ht="48" x14ac:dyDescent="0.2">
       <c r="B12" s="11" t="s">
         <v>13</v>
       </c>
@@ -1259,8 +1309,12 @@
       <c r="F12" s="15" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="13" spans="2:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G12" s="14"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="15"/>
+    </row>
+    <row r="13" spans="2:10" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B13" s="16" t="s">
         <v>14</v>
       </c>
@@ -1276,20 +1330,26 @@
       <c r="F13" s="24" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="G13" s="19"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="24"/>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C16" t="s">
         <v>38</v>
       </c>
-      <c r="D16" s="45">
+      <c r="D16" s="39">
         <f>C9+C10+C11+C12+C13+E9+E10+E11+E12+E13</f>
         <v>61</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="I7:J7"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -1304,50 +1364,50 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.453125"/>
-    <col min="2" max="2" width="13.453125"/>
-    <col min="3" max="3" width="12.1796875"/>
-    <col min="4" max="4" width="39.81640625"/>
-    <col min="5" max="5" width="10.36328125"/>
-    <col min="6" max="6" width="40.453125" customWidth="1"/>
-    <col min="7" max="7" width="9.453125"/>
-    <col min="8" max="8" width="39.81640625"/>
-    <col min="9" max="254" width="9.453125"/>
-    <col min="255" max="1023" width="11.453125"/>
+    <col min="1" max="1" width="9.5"/>
+    <col min="2" max="2" width="13.5"/>
+    <col min="3" max="3" width="12.1640625"/>
+    <col min="4" max="4" width="39.83203125"/>
+    <col min="5" max="5" width="10.33203125"/>
+    <col min="6" max="6" width="40.5" customWidth="1"/>
+    <col min="7" max="7" width="9.5"/>
+    <col min="8" max="8" width="39.83203125"/>
+    <col min="9" max="254" width="9.5"/>
+    <col min="255" max="1023" width="11.5"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="2:8" ht="24" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:8" ht="19" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="2:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="30" t="s">
+    <row r="6" spans="2:8" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="2:8" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="C7" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="30"/>
-      <c r="E7" s="31" t="s">
+      <c r="D7" s="40"/>
+      <c r="E7" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="31"/>
-      <c r="G7" s="32" t="s">
+      <c r="F7" s="43"/>
+      <c r="G7" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="H7" s="33"/>
-    </row>
-    <row r="8" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H7" s="42"/>
+    </row>
+    <row r="8" spans="2:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C8" s="3" t="s">
         <v>4</v>
       </c>
@@ -1367,7 +1427,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="58.5" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:8" ht="49" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
         <v>6</v>
       </c>
@@ -1386,7 +1446,7 @@
       <c r="G9" s="9"/>
       <c r="H9" s="22"/>
     </row>
-    <row r="10" spans="2:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:8" ht="32" x14ac:dyDescent="0.2">
       <c r="B10" s="11" t="s">
         <v>9</v>
       </c>
@@ -1405,7 +1465,7 @@
       <c r="G10" s="14"/>
       <c r="H10" s="15"/>
     </row>
-    <row r="11" spans="2:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:8" ht="64" x14ac:dyDescent="0.2">
       <c r="B11" s="11" t="s">
         <v>10</v>
       </c>
@@ -1424,7 +1484,7 @@
       <c r="G11" s="14"/>
       <c r="H11" s="15"/>
     </row>
-    <row r="12" spans="2:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:8" ht="32" x14ac:dyDescent="0.2">
       <c r="B12" s="11" t="s">
         <v>13</v>
       </c>
@@ -1443,7 +1503,7 @@
       <c r="G12" s="14"/>
       <c r="H12" s="15"/>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B13" s="25" t="s">
         <v>28</v>
       </c>
@@ -1458,7 +1518,7 @@
       <c r="G13" s="28"/>
       <c r="H13" s="29"/>
     </row>
-    <row r="14" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B14" s="16" t="s">
         <v>14</v>
       </c>
@@ -1492,61 +1552,61 @@
       <selection activeCell="P7" sqref="P7:P12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="13.36328125" customWidth="1"/>
-    <col min="4" max="4" width="39.26953125" customWidth="1"/>
-    <col min="5" max="5" width="13.36328125" customWidth="1"/>
-    <col min="6" max="6" width="39.26953125" customWidth="1"/>
-    <col min="7" max="7" width="13.26953125" customWidth="1"/>
-    <col min="8" max="8" width="39.26953125" customWidth="1"/>
-    <col min="9" max="9" width="13.26953125" customWidth="1"/>
-    <col min="10" max="10" width="39.26953125" customWidth="1"/>
-    <col min="11" max="11" width="13.26953125" customWidth="1"/>
-    <col min="12" max="12" width="39.26953125" customWidth="1"/>
-    <col min="13" max="13" width="13.26953125" customWidth="1"/>
-    <col min="14" max="14" width="39.26953125" customWidth="1"/>
-    <col min="15" max="15" width="13.26953125" customWidth="1"/>
-    <col min="16" max="16" width="39.26953125" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" customWidth="1"/>
+    <col min="4" max="4" width="39.33203125" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" customWidth="1"/>
+    <col min="6" max="6" width="39.33203125" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" customWidth="1"/>
+    <col min="8" max="8" width="39.33203125" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" customWidth="1"/>
+    <col min="10" max="10" width="39.33203125" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" customWidth="1"/>
+    <col min="12" max="12" width="39.33203125" customWidth="1"/>
+    <col min="13" max="13" width="13.33203125" customWidth="1"/>
+    <col min="14" max="14" width="39.33203125" customWidth="1"/>
+    <col min="15" max="15" width="13.33203125" customWidth="1"/>
+    <col min="16" max="16" width="39.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:16" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:16" ht="19" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="5" spans="2:16" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="C5" s="34" t="s">
+    <row r="4" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="2:16" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="C5" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="30"/>
-      <c r="E5" s="34">
+      <c r="D5" s="40"/>
+      <c r="E5" s="45">
         <v>43430</v>
       </c>
-      <c r="F5" s="30"/>
-      <c r="G5" s="35">
+      <c r="F5" s="40"/>
+      <c r="G5" s="44">
         <v>43431</v>
       </c>
-      <c r="H5" s="31"/>
-      <c r="I5" s="35">
+      <c r="H5" s="43"/>
+      <c r="I5" s="44">
         <v>43432</v>
       </c>
-      <c r="J5" s="31"/>
-      <c r="K5" s="35">
+      <c r="J5" s="43"/>
+      <c r="K5" s="44">
         <v>43433</v>
       </c>
-      <c r="L5" s="31"/>
-      <c r="M5" s="35">
+      <c r="L5" s="43"/>
+      <c r="M5" s="44">
         <v>43434</v>
       </c>
-      <c r="N5" s="31"/>
-      <c r="O5" s="35" t="s">
+      <c r="N5" s="43"/>
+      <c r="O5" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="P5" s="31"/>
-    </row>
-    <row r="6" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="P5" s="43"/>
+    </row>
+    <row r="6" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C6" s="3" t="s">
         <v>4</v>
       </c>
@@ -1590,12 +1650,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="2:16" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:16" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B7" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="7"/>
-      <c r="D7" s="36"/>
+      <c r="D7" s="30"/>
       <c r="E7" s="7"/>
       <c r="F7" s="8"/>
       <c r="G7" s="9"/>
@@ -1609,90 +1669,90 @@
       <c r="O7" s="9"/>
       <c r="P7" s="10"/>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B8" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="12"/>
-      <c r="D8" s="37"/>
+      <c r="D8" s="31"/>
       <c r="E8" s="12"/>
-      <c r="F8" s="40"/>
+      <c r="F8" s="34"/>
       <c r="G8" s="14"/>
-      <c r="H8" s="43"/>
+      <c r="H8" s="37"/>
       <c r="I8" s="14"/>
-      <c r="J8" s="43"/>
+      <c r="J8" s="37"/>
       <c r="K8" s="14"/>
-      <c r="L8" s="43"/>
+      <c r="L8" s="37"/>
       <c r="M8" s="14"/>
-      <c r="N8" s="43"/>
+      <c r="N8" s="37"/>
       <c r="O8" s="14"/>
-      <c r="P8" s="43"/>
-    </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="P8" s="37"/>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B9" s="11" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="12"/>
-      <c r="D9" s="37"/>
+      <c r="D9" s="31"/>
       <c r="E9" s="12"/>
-      <c r="F9" s="40"/>
+      <c r="F9" s="34"/>
       <c r="G9" s="14"/>
-      <c r="H9" s="43"/>
+      <c r="H9" s="37"/>
       <c r="I9" s="14"/>
-      <c r="J9" s="43"/>
+      <c r="J9" s="37"/>
       <c r="K9" s="14"/>
-      <c r="L9" s="43"/>
+      <c r="L9" s="37"/>
       <c r="M9" s="14"/>
-      <c r="N9" s="43"/>
+      <c r="N9" s="37"/>
       <c r="O9" s="14"/>
-      <c r="P9" s="43"/>
-    </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="P9" s="37"/>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B10" s="11" t="s">
         <v>13</v>
       </c>
       <c r="C10" s="12"/>
-      <c r="D10" s="37"/>
+      <c r="D10" s="31"/>
       <c r="E10" s="12"/>
-      <c r="F10" s="40"/>
+      <c r="F10" s="34"/>
       <c r="G10" s="14"/>
-      <c r="H10" s="43"/>
+      <c r="H10" s="37"/>
       <c r="I10" s="14"/>
-      <c r="J10" s="43"/>
+      <c r="J10" s="37"/>
       <c r="K10" s="14"/>
-      <c r="L10" s="43"/>
+      <c r="L10" s="37"/>
       <c r="M10" s="14"/>
-      <c r="N10" s="43"/>
+      <c r="N10" s="37"/>
       <c r="O10" s="14"/>
-      <c r="P10" s="43"/>
-    </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="P10" s="37"/>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B11" s="25" t="s">
         <v>28</v>
       </c>
       <c r="C11" s="26"/>
-      <c r="D11" s="38"/>
+      <c r="D11" s="32"/>
       <c r="E11" s="26"/>
-      <c r="F11" s="41"/>
+      <c r="F11" s="35"/>
       <c r="G11" s="28"/>
-      <c r="H11" s="44"/>
+      <c r="H11" s="38"/>
       <c r="I11" s="28"/>
-      <c r="J11" s="44"/>
+      <c r="J11" s="38"/>
       <c r="K11" s="28"/>
-      <c r="L11" s="44"/>
+      <c r="L11" s="38"/>
       <c r="M11" s="28"/>
-      <c r="N11" s="44"/>
+      <c r="N11" s="38"/>
       <c r="O11" s="28"/>
-      <c r="P11" s="44"/>
-    </row>
-    <row r="12" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="P11" s="38"/>
+    </row>
+    <row r="12" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="16" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="17"/>
-      <c r="D12" s="39"/>
+      <c r="D12" s="33"/>
       <c r="E12" s="17"/>
-      <c r="F12" s="42"/>
+      <c r="F12" s="36"/>
       <c r="G12" s="19"/>
       <c r="H12" s="24"/>
       <c r="I12" s="19"/>

</xml_diff>

<commit_message>
ILV.xlsx Heute 5h gearbeitet.
Siehe vorhergehende commits.
</commit_message>
<xml_diff>
--- a/ILV.xlsx
+++ b/ILV.xlsx
@@ -1,28 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carme\Documents\GitHub\Pro1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/frank/Pro1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{080D0940-B320-4938-86F8-F7346A778D35}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E68BF8EB-555D-6B46-9AEB-E7F16829F44A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="22425" windowHeight="14625" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="22420" windowHeight="14620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Recherche-Dokument" sheetId="1" r:id="rId1"/>
     <sheet name="Pflichtenheft org." sheetId="2" r:id="rId2"/>
     <sheet name="Pflichtenheft techn." sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="47">
   <si>
     <t>ILV</t>
   </si>
@@ -181,6 +181,15 @@
   </si>
   <si>
     <t>1.5</t>
+  </si>
+  <si>
+    <t>5h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pflichtenheft Risikoanalyse Bildqualität verbessern
+Projektstrukturplantabellen -&gt; LateX
+Projektbudgettabelle vervollstaendigt
+</t>
   </si>
 </sst>
 </file>
@@ -1164,34 +1173,34 @@
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.42578125"/>
-    <col min="2" max="2" width="13.42578125"/>
-    <col min="3" max="3" width="12.140625"/>
-    <col min="4" max="4" width="38.7109375" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625"/>
-    <col min="6" max="6" width="38.7109375" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125"/>
-    <col min="8" max="8" width="38.7109375" customWidth="1"/>
-    <col min="9" max="9" width="9.42578125"/>
-    <col min="10" max="10" width="28.42578125" customWidth="1"/>
-    <col min="11" max="256" width="9.42578125"/>
-    <col min="257" max="1025" width="11.42578125"/>
+    <col min="1" max="1" width="9.5"/>
+    <col min="2" max="2" width="13.5"/>
+    <col min="3" max="3" width="12.1640625"/>
+    <col min="4" max="4" width="38.6640625" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125"/>
+    <col min="6" max="6" width="38.6640625" customWidth="1"/>
+    <col min="7" max="7" width="9.5"/>
+    <col min="8" max="8" width="38.6640625" customWidth="1"/>
+    <col min="9" max="9" width="9.5"/>
+    <col min="10" max="10" width="28.5" customWidth="1"/>
+    <col min="11" max="256" width="9.5"/>
+    <col min="257" max="1025" width="11.5"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:10" ht="24" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" ht="19" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="2:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="2:10" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="C7" s="40" t="s">
         <v>2</v>
       </c>
@@ -1209,7 +1218,7 @@
       </c>
       <c r="J7" s="42"/>
     </row>
-    <row r="8" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C8" s="3" t="s">
         <v>4</v>
       </c>
@@ -1235,7 +1244,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="2:10" ht="105.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10" ht="97" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
         <v>6</v>
       </c>
@@ -1256,7 +1265,7 @@
       <c r="I9" s="9"/>
       <c r="J9" s="10"/>
     </row>
-    <row r="10" spans="2:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:10" ht="48" x14ac:dyDescent="0.2">
       <c r="B10" s="11" t="s">
         <v>9</v>
       </c>
@@ -1277,7 +1286,7 @@
       <c r="I10" s="14"/>
       <c r="J10" s="15"/>
     </row>
-    <row r="11" spans="2:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10" ht="48" x14ac:dyDescent="0.2">
       <c r="B11" s="11" t="s">
         <v>10</v>
       </c>
@@ -1302,7 +1311,7 @@
       <c r="I11" s="14"/>
       <c r="J11" s="15"/>
     </row>
-    <row r="12" spans="2:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10" ht="48" x14ac:dyDescent="0.2">
       <c r="B12" s="11" t="s">
         <v>13</v>
       </c>
@@ -1323,7 +1332,7 @@
       <c r="I12" s="14"/>
       <c r="J12" s="15"/>
     </row>
-    <row r="13" spans="2:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:10" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B13" s="16" t="s">
         <v>14</v>
       </c>
@@ -1344,7 +1353,7 @@
       <c r="I13" s="19"/>
       <c r="J13" s="24"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C16" t="s">
         <v>38</v>
       </c>
@@ -1373,36 +1382,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.42578125"/>
-    <col min="2" max="2" width="13.42578125"/>
-    <col min="3" max="3" width="12.140625"/>
-    <col min="4" max="4" width="39.85546875"/>
-    <col min="5" max="5" width="10.28515625"/>
-    <col min="6" max="6" width="40.42578125" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125"/>
-    <col min="8" max="8" width="39.85546875"/>
-    <col min="9" max="254" width="9.42578125"/>
-    <col min="255" max="1023" width="11.42578125"/>
+    <col min="1" max="1" width="9.5"/>
+    <col min="2" max="2" width="13.5"/>
+    <col min="3" max="3" width="12.1640625"/>
+    <col min="4" max="4" width="39.83203125"/>
+    <col min="5" max="5" width="10.33203125"/>
+    <col min="6" max="6" width="40.5" customWidth="1"/>
+    <col min="7" max="7" width="9.5"/>
+    <col min="8" max="8" width="39.83203125"/>
+    <col min="9" max="254" width="9.5"/>
+    <col min="255" max="1023" width="11.5"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:8" ht="24" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:8" ht="19" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="2:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="2:8" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="C7" s="40" t="s">
         <v>15</v>
       </c>
@@ -1416,7 +1425,7 @@
       </c>
       <c r="H7" s="42"/>
     </row>
-    <row r="8" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C8" s="3" t="s">
         <v>4</v>
       </c>
@@ -1436,7 +1445,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="60.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" ht="49" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
         <v>6</v>
       </c>
@@ -1455,7 +1464,7 @@
       <c r="G9" s="9"/>
       <c r="H9" s="22"/>
     </row>
-    <row r="10" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:8" ht="32" x14ac:dyDescent="0.2">
       <c r="B10" s="11" t="s">
         <v>9</v>
       </c>
@@ -1474,7 +1483,7 @@
       <c r="G10" s="14"/>
       <c r="H10" s="15"/>
     </row>
-    <row r="11" spans="2:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:8" ht="64" x14ac:dyDescent="0.2">
       <c r="B11" s="11" t="s">
         <v>10</v>
       </c>
@@ -1490,10 +1499,14 @@
       <c r="F11" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="G11" s="14"/>
-      <c r="H11" s="15"/>
-    </row>
-    <row r="12" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="G11" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="H11" s="15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" ht="32" x14ac:dyDescent="0.2">
       <c r="B12" s="11" t="s">
         <v>13</v>
       </c>
@@ -1512,7 +1525,7 @@
       <c r="G12" s="14"/>
       <c r="H12" s="15"/>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B13" s="25" t="s">
         <v>28</v>
       </c>
@@ -1527,7 +1540,7 @@
       <c r="G13" s="28"/>
       <c r="H13" s="29"/>
     </row>
-    <row r="14" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B14" s="16" t="s">
         <v>14</v>
       </c>
@@ -1569,31 +1582,31 @@
       <selection activeCell="P7" sqref="P7:P12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="13.28515625" customWidth="1"/>
-    <col min="4" max="4" width="39.28515625" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" customWidth="1"/>
-    <col min="6" max="6" width="39.28515625" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" customWidth="1"/>
-    <col min="8" max="8" width="39.28515625" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" customWidth="1"/>
-    <col min="10" max="10" width="39.28515625" customWidth="1"/>
-    <col min="11" max="11" width="13.28515625" customWidth="1"/>
-    <col min="12" max="12" width="39.28515625" customWidth="1"/>
-    <col min="13" max="13" width="13.28515625" customWidth="1"/>
-    <col min="14" max="14" width="39.28515625" customWidth="1"/>
-    <col min="15" max="15" width="13.28515625" customWidth="1"/>
-    <col min="16" max="16" width="39.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" customWidth="1"/>
+    <col min="4" max="4" width="39.33203125" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" customWidth="1"/>
+    <col min="6" max="6" width="39.33203125" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" customWidth="1"/>
+    <col min="8" max="8" width="39.33203125" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" customWidth="1"/>
+    <col min="10" max="10" width="39.33203125" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" customWidth="1"/>
+    <col min="12" max="12" width="39.33203125" customWidth="1"/>
+    <col min="13" max="13" width="13.33203125" customWidth="1"/>
+    <col min="14" max="14" width="39.33203125" customWidth="1"/>
+    <col min="15" max="15" width="13.33203125" customWidth="1"/>
+    <col min="16" max="16" width="39.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:16" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:16" ht="19" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="2:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="2:16" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="C5" s="45" t="s">
         <v>37</v>
       </c>
@@ -1623,7 +1636,7 @@
       </c>
       <c r="P5" s="43"/>
     </row>
-    <row r="6" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C6" s="3" t="s">
         <v>4</v>
       </c>
@@ -1667,7 +1680,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="2:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:16" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B7" s="6" t="s">
         <v>6</v>
       </c>
@@ -1686,7 +1699,7 @@
       <c r="O7" s="9"/>
       <c r="P7" s="10"/>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B8" s="11" t="s">
         <v>9</v>
       </c>
@@ -1705,7 +1718,7 @@
       <c r="O8" s="14"/>
       <c r="P8" s="37"/>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B9" s="11" t="s">
         <v>10</v>
       </c>
@@ -1724,7 +1737,7 @@
       <c r="O9" s="14"/>
       <c r="P9" s="37"/>
     </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B10" s="11" t="s">
         <v>13</v>
       </c>
@@ -1743,7 +1756,7 @@
       <c r="O10" s="14"/>
       <c r="P10" s="37"/>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B11" s="25" t="s">
         <v>28</v>
       </c>
@@ -1762,7 +1775,7 @@
       <c r="O11" s="28"/>
       <c r="P11" s="38"/>
     </row>
-    <row r="12" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="16" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
Update ILV.xlsx Riskioanalyse Zeit hinzugefügt
</commit_message>
<xml_diff>
--- a/ILV.xlsx
+++ b/ILV.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/frank/Pro1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ramiro18/Library/Group Containers/UBF8T346G9.ms/MerpTempItems/Schule/Studium/Pro1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E68BF8EB-555D-6B46-9AEB-E7F16829F44A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABD50893-9999-7A4A-85C0-A093DAA240B6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="22420" windowHeight="14620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Pflichtenheft org." sheetId="2" r:id="rId2"/>
     <sheet name="Pflichtenheft techn." sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -183,13 +183,13 @@
     <t>1.5</t>
   </si>
   <si>
-    <t>5h</t>
-  </si>
-  <si>
     <t xml:space="preserve">Pflichtenheft Risikoanalyse Bildqualität verbessern
 Projektstrukturplantabellen -&gt; LateX
 Projektbudgettabelle vervollstaendigt
 </t>
+  </si>
+  <si>
+    <t>Risikoanalysetabelle erstellen</t>
   </si>
 </sst>
 </file>
@@ -787,7 +787,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -871,7 +871,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1383,7 +1383,7 @@
   <dimension ref="B2:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1480,8 +1480,12 @@
       <c r="F10" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="G10" s="14"/>
-      <c r="H10" s="15"/>
+      <c r="G10" s="14">
+        <v>2</v>
+      </c>
+      <c r="H10" s="15" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="11" spans="2:8" ht="64" x14ac:dyDescent="0.2">
       <c r="B11" s="11" t="s">
@@ -1499,11 +1503,11 @@
       <c r="F11" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="G11" s="14" t="s">
+      <c r="G11" s="14">
+        <v>5</v>
+      </c>
+      <c r="H11" s="15" t="s">
         <v>45</v>
-      </c>
-      <c r="H11" s="15" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="12" spans="2:8" ht="32" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
update ILV.tex Grobkonzept teil1
</commit_message>
<xml_diff>
--- a/ILV.xlsx
+++ b/ILV.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\i00202920\Documents\GitHub\Pro1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ramiro18/Library/Group Containers/UBF8T346G9.ms/MerpTempItems/Schule/Studium/Pro1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{77BB2426-A910-4F3C-8AD4-28F2E3A335A3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BD226B7-4A12-7A47-869B-08509854B674}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="22420" windowHeight="14620" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,12 +17,12 @@
     <sheet name="Pflichtenheft org." sheetId="2" r:id="rId2"/>
     <sheet name="Pflichtenheft techn." sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="49">
   <si>
     <t>ILV</t>
   </si>
@@ -196,6 +196,9 @@
 - Kleinere Korrekturen(0.8h) + Batchdatei (0.2h)
 - KIS (1h)
 - Auswertung (1.5h)</t>
+  </si>
+  <si>
+    <t>Mindmap(2h),  Grobkonzept(5.5)</t>
   </si>
 </sst>
 </file>
@@ -1179,34 +1182,34 @@
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.453125"/>
-    <col min="2" max="2" width="13.453125"/>
-    <col min="3" max="3" width="12.1796875"/>
-    <col min="4" max="4" width="38.6328125" customWidth="1"/>
-    <col min="5" max="5" width="10.36328125"/>
-    <col min="6" max="6" width="38.6328125" customWidth="1"/>
-    <col min="7" max="7" width="9.453125"/>
-    <col min="8" max="8" width="38.6328125" customWidth="1"/>
-    <col min="9" max="9" width="9.453125"/>
-    <col min="10" max="10" width="28.453125" customWidth="1"/>
-    <col min="11" max="256" width="9.453125"/>
-    <col min="257" max="1025" width="11.453125"/>
+    <col min="1" max="1" width="9.5"/>
+    <col min="2" max="2" width="13.5"/>
+    <col min="3" max="3" width="12.1640625"/>
+    <col min="4" max="4" width="38.6640625" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125"/>
+    <col min="6" max="6" width="38.6640625" customWidth="1"/>
+    <col min="7" max="7" width="9.5"/>
+    <col min="8" max="8" width="38.6640625" customWidth="1"/>
+    <col min="9" max="9" width="9.5"/>
+    <col min="10" max="10" width="28.5" customWidth="1"/>
+    <col min="11" max="256" width="9.5"/>
+    <col min="257" max="1025" width="11.5"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="2:10" ht="24" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:10" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:10" ht="19" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="2:10" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="2:10" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="C7" s="40" t="s">
         <v>2</v>
       </c>
@@ -1224,7 +1227,7 @@
       </c>
       <c r="J7" s="42"/>
     </row>
-    <row r="8" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C8" s="3" t="s">
         <v>4</v>
       </c>
@@ -1250,7 +1253,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="2:10" ht="102" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:10" ht="97" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
         <v>6</v>
       </c>
@@ -1271,7 +1274,7 @@
       <c r="I9" s="9"/>
       <c r="J9" s="10"/>
     </row>
-    <row r="10" spans="2:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:10" ht="48" x14ac:dyDescent="0.2">
       <c r="B10" s="11" t="s">
         <v>9</v>
       </c>
@@ -1292,7 +1295,7 @@
       <c r="I10" s="14"/>
       <c r="J10" s="15"/>
     </row>
-    <row r="11" spans="2:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:10" ht="48" x14ac:dyDescent="0.2">
       <c r="B11" s="11" t="s">
         <v>10</v>
       </c>
@@ -1317,7 +1320,7 @@
       <c r="I11" s="14"/>
       <c r="J11" s="15"/>
     </row>
-    <row r="12" spans="2:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:10" ht="48" x14ac:dyDescent="0.2">
       <c r="B12" s="11" t="s">
         <v>13</v>
       </c>
@@ -1338,7 +1341,7 @@
       <c r="I12" s="14"/>
       <c r="J12" s="15"/>
     </row>
-    <row r="13" spans="2:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:10" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B13" s="16" t="s">
         <v>14</v>
       </c>
@@ -1359,7 +1362,7 @@
       <c r="I13" s="19"/>
       <c r="J13" s="24"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C16" t="s">
         <v>38</v>
       </c>
@@ -1392,32 +1395,32 @@
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.453125"/>
-    <col min="2" max="2" width="13.453125"/>
-    <col min="3" max="3" width="12.1796875"/>
-    <col min="4" max="4" width="39.81640625"/>
-    <col min="5" max="5" width="10.36328125"/>
-    <col min="6" max="6" width="40.453125" customWidth="1"/>
-    <col min="7" max="7" width="9.453125"/>
-    <col min="8" max="8" width="39.81640625"/>
-    <col min="9" max="254" width="9.453125"/>
-    <col min="255" max="1023" width="11.453125"/>
+    <col min="1" max="1" width="9.5"/>
+    <col min="2" max="2" width="13.5"/>
+    <col min="3" max="3" width="12.1640625"/>
+    <col min="4" max="4" width="39.83203125"/>
+    <col min="5" max="5" width="10.33203125"/>
+    <col min="6" max="6" width="40.5" customWidth="1"/>
+    <col min="7" max="7" width="9.5"/>
+    <col min="8" max="8" width="39.83203125"/>
+    <col min="9" max="254" width="9.5"/>
+    <col min="255" max="1023" width="11.5"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="2:8" ht="24" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:8" ht="19" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="2:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:8" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="2:8" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="C7" s="40" t="s">
         <v>15</v>
       </c>
@@ -1431,7 +1434,7 @@
       </c>
       <c r="H7" s="42"/>
     </row>
-    <row r="8" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C8" s="3" t="s">
         <v>4</v>
       </c>
@@ -1451,7 +1454,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="58.5" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:8" ht="49" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
         <v>6</v>
       </c>
@@ -1470,7 +1473,7 @@
       <c r="G9" s="9"/>
       <c r="H9" s="22"/>
     </row>
-    <row r="10" spans="2:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:8" ht="32" x14ac:dyDescent="0.2">
       <c r="B10" s="11" t="s">
         <v>9</v>
       </c>
@@ -1493,7 +1496,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="2:8" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:8" ht="64" x14ac:dyDescent="0.2">
       <c r="B11" s="11" t="s">
         <v>10</v>
       </c>
@@ -1516,7 +1519,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="2:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:8" ht="32" x14ac:dyDescent="0.2">
       <c r="B12" s="11" t="s">
         <v>13</v>
       </c>
@@ -1535,7 +1538,7 @@
       <c r="G12" s="14"/>
       <c r="H12" s="15"/>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B13" s="25" t="s">
         <v>28</v>
       </c>
@@ -1550,7 +1553,7 @@
       <c r="G13" s="28"/>
       <c r="H13" s="29"/>
     </row>
-    <row r="14" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B14" s="16" t="s">
         <v>14</v>
       </c>
@@ -1589,34 +1592,34 @@
   <dimension ref="B3:P12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="13.36328125" customWidth="1"/>
-    <col min="4" max="4" width="40.54296875" customWidth="1"/>
-    <col min="5" max="5" width="13.36328125" customWidth="1"/>
-    <col min="6" max="6" width="39.36328125" customWidth="1"/>
-    <col min="7" max="7" width="13.36328125" customWidth="1"/>
-    <col min="8" max="8" width="39.36328125" customWidth="1"/>
-    <col min="9" max="9" width="13.36328125" customWidth="1"/>
-    <col min="10" max="10" width="39.36328125" customWidth="1"/>
-    <col min="11" max="11" width="13.36328125" customWidth="1"/>
-    <col min="12" max="12" width="39.36328125" customWidth="1"/>
-    <col min="13" max="13" width="13.36328125" customWidth="1"/>
-    <col min="14" max="14" width="39.36328125" customWidth="1"/>
-    <col min="15" max="15" width="13.36328125" customWidth="1"/>
-    <col min="16" max="16" width="39.36328125" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" customWidth="1"/>
+    <col min="4" max="4" width="40.5" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" customWidth="1"/>
+    <col min="6" max="6" width="39.33203125" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" customWidth="1"/>
+    <col min="8" max="8" width="39.33203125" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" customWidth="1"/>
+    <col min="10" max="10" width="39.33203125" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" customWidth="1"/>
+    <col min="12" max="12" width="39.33203125" customWidth="1"/>
+    <col min="13" max="13" width="13.33203125" customWidth="1"/>
+    <col min="14" max="14" width="39.33203125" customWidth="1"/>
+    <col min="15" max="15" width="13.33203125" customWidth="1"/>
+    <col min="16" max="16" width="39.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:16" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:16" ht="19" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="5" spans="2:16" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="2:16" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="C5" s="45" t="s">
         <v>37</v>
       </c>
@@ -1646,7 +1649,7 @@
       </c>
       <c r="P5" s="43"/>
     </row>
-    <row r="6" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C6" s="3" t="s">
         <v>4</v>
       </c>
@@ -1690,7 +1693,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="2:16" ht="58.5" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:16" ht="65" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B7" s="6" t="s">
         <v>6</v>
       </c>
@@ -1713,14 +1716,16 @@
       <c r="O7" s="9"/>
       <c r="P7" s="10"/>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:16" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="12"/>
       <c r="D8" s="31"/>
       <c r="E8" s="12"/>
-      <c r="F8" s="34"/>
+      <c r="F8" s="34" t="s">
+        <v>48</v>
+      </c>
       <c r="G8" s="14"/>
       <c r="H8" s="37"/>
       <c r="I8" s="14"/>
@@ -1732,7 +1737,7 @@
       <c r="O8" s="14"/>
       <c r="P8" s="37"/>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B9" s="11" t="s">
         <v>10</v>
       </c>
@@ -1751,7 +1756,7 @@
       <c r="O9" s="14"/>
       <c r="P9" s="37"/>
     </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B10" s="11" t="s">
         <v>13</v>
       </c>
@@ -1770,7 +1775,7 @@
       <c r="O10" s="14"/>
       <c r="P10" s="37"/>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B11" s="25" t="s">
         <v>28</v>
       </c>
@@ -1789,7 +1794,7 @@
       <c r="O11" s="28"/>
       <c r="P11" s="38"/>
     </row>
-    <row r="12" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="16" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
ILV Arbeit mo nachmittag
</commit_message>
<xml_diff>
--- a/ILV.xlsx
+++ b/ILV.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ramiro18/Library/Group Containers/UBF8T346G9.ms/MerpTempItems/Schule/Studium/Pro1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\i00202920\Documents\GitHub\Pro1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BD226B7-4A12-7A47-869B-08509854B674}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{AC3E5224-F3CB-498F-96DD-ECAEBDD471BD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="22420" windowHeight="14620" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Pflichtenheft org." sheetId="2" r:id="rId2"/>
     <sheet name="Pflichtenheft techn." sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
@@ -192,13 +192,13 @@
     <t>Risikoanalysetabelle erstellen</t>
   </si>
   <si>
+    <t>Mindmap(2h),  Grobkonzept(5.5)</t>
+  </si>
+  <si>
     <t>-Grundstruktur (1h)
 - Kleinere Korrekturen(0.8h) + Batchdatei (0.2h)
 - KIS (1h)
-- Auswertung (1.5h)</t>
-  </si>
-  <si>
-    <t>Mindmap(2h),  Grobkonzept(5.5)</t>
+- Auswertung (4.5h)</t>
   </si>
 </sst>
 </file>
@@ -1182,34 +1182,34 @@
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.5"/>
-    <col min="2" max="2" width="13.5"/>
-    <col min="3" max="3" width="12.1640625"/>
-    <col min="4" max="4" width="38.6640625" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125"/>
-    <col min="6" max="6" width="38.6640625" customWidth="1"/>
-    <col min="7" max="7" width="9.5"/>
-    <col min="8" max="8" width="38.6640625" customWidth="1"/>
-    <col min="9" max="9" width="9.5"/>
-    <col min="10" max="10" width="28.5" customWidth="1"/>
-    <col min="11" max="256" width="9.5"/>
-    <col min="257" max="1025" width="11.5"/>
+    <col min="1" max="1" width="9.453125"/>
+    <col min="2" max="2" width="13.453125"/>
+    <col min="3" max="3" width="12.1796875"/>
+    <col min="4" max="4" width="38.6328125" customWidth="1"/>
+    <col min="5" max="5" width="10.36328125"/>
+    <col min="6" max="6" width="38.6328125" customWidth="1"/>
+    <col min="7" max="7" width="9.453125"/>
+    <col min="8" max="8" width="38.6328125" customWidth="1"/>
+    <col min="9" max="9" width="9.453125"/>
+    <col min="10" max="10" width="28.453125" customWidth="1"/>
+    <col min="11" max="256" width="9.453125"/>
+    <col min="257" max="1025" width="11.453125"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" ht="24" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:10" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:10" ht="19" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="2:10" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="7" spans="2:10" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="C7" s="40" t="s">
         <v>2</v>
       </c>
@@ -1227,7 +1227,7 @@
       </c>
       <c r="J7" s="42"/>
     </row>
-    <row r="8" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C8" s="3" t="s">
         <v>4</v>
       </c>
@@ -1253,7 +1253,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="2:10" ht="97" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:10" ht="102" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B9" s="6" t="s">
         <v>6</v>
       </c>
@@ -1274,7 +1274,7 @@
       <c r="I9" s="9"/>
       <c r="J9" s="10"/>
     </row>
-    <row r="10" spans="2:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B10" s="11" t="s">
         <v>9</v>
       </c>
@@ -1295,7 +1295,7 @@
       <c r="I10" s="14"/>
       <c r="J10" s="15"/>
     </row>
-    <row r="11" spans="2:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B11" s="11" t="s">
         <v>10</v>
       </c>
@@ -1320,7 +1320,7 @@
       <c r="I11" s="14"/>
       <c r="J11" s="15"/>
     </row>
-    <row r="12" spans="2:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B12" s="11" t="s">
         <v>13</v>
       </c>
@@ -1341,7 +1341,7 @@
       <c r="I12" s="14"/>
       <c r="J12" s="15"/>
     </row>
-    <row r="13" spans="2:10" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B13" s="16" t="s">
         <v>14</v>
       </c>
@@ -1362,7 +1362,7 @@
       <c r="I13" s="19"/>
       <c r="J13" s="24"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
       <c r="C16" t="s">
         <v>38</v>
       </c>
@@ -1395,32 +1395,32 @@
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.5"/>
-    <col min="2" max="2" width="13.5"/>
-    <col min="3" max="3" width="12.1640625"/>
-    <col min="4" max="4" width="39.83203125"/>
-    <col min="5" max="5" width="10.33203125"/>
-    <col min="6" max="6" width="40.5" customWidth="1"/>
-    <col min="7" max="7" width="9.5"/>
-    <col min="8" max="8" width="39.83203125"/>
-    <col min="9" max="254" width="9.5"/>
-    <col min="255" max="1023" width="11.5"/>
+    <col min="1" max="1" width="9.453125"/>
+    <col min="2" max="2" width="13.453125"/>
+    <col min="3" max="3" width="12.1796875"/>
+    <col min="4" max="4" width="39.81640625"/>
+    <col min="5" max="5" width="10.36328125"/>
+    <col min="6" max="6" width="40.453125" customWidth="1"/>
+    <col min="7" max="7" width="9.453125"/>
+    <col min="8" max="8" width="39.81640625"/>
+    <col min="9" max="254" width="9.453125"/>
+    <col min="255" max="1023" width="11.453125"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="24" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:8" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B5" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="2:8" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="7" spans="2:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="C7" s="40" t="s">
         <v>15</v>
       </c>
@@ -1434,7 +1434,7 @@
       </c>
       <c r="H7" s="42"/>
     </row>
-    <row r="8" spans="2:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C8" s="3" t="s">
         <v>4</v>
       </c>
@@ -1454,7 +1454,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="49" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:8" ht="58.5" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B9" s="6" t="s">
         <v>6</v>
       </c>
@@ -1473,7 +1473,7 @@
       <c r="G9" s="9"/>
       <c r="H9" s="22"/>
     </row>
-    <row r="10" spans="2:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:8" ht="29" x14ac:dyDescent="0.35">
       <c r="B10" s="11" t="s">
         <v>9</v>
       </c>
@@ -1496,7 +1496,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="2:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B11" s="11" t="s">
         <v>10</v>
       </c>
@@ -1519,7 +1519,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="2:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:8" ht="29" x14ac:dyDescent="0.35">
       <c r="B12" s="11" t="s">
         <v>13</v>
       </c>
@@ -1538,7 +1538,7 @@
       <c r="G12" s="14"/>
       <c r="H12" s="15"/>
     </row>
-    <row r="13" spans="2:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B13" s="25" t="s">
         <v>28</v>
       </c>
@@ -1553,7 +1553,7 @@
       <c r="G13" s="28"/>
       <c r="H13" s="29"/>
     </row>
-    <row r="14" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B14" s="16" t="s">
         <v>14</v>
       </c>
@@ -1592,34 +1592,34 @@
   <dimension ref="B3:P12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="13.33203125" customWidth="1"/>
-    <col min="4" max="4" width="40.5" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" customWidth="1"/>
-    <col min="6" max="6" width="39.33203125" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" customWidth="1"/>
-    <col min="8" max="8" width="39.33203125" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" customWidth="1"/>
-    <col min="10" max="10" width="39.33203125" customWidth="1"/>
-    <col min="11" max="11" width="13.33203125" customWidth="1"/>
-    <col min="12" max="12" width="39.33203125" customWidth="1"/>
-    <col min="13" max="13" width="13.33203125" customWidth="1"/>
-    <col min="14" max="14" width="39.33203125" customWidth="1"/>
-    <col min="15" max="15" width="13.33203125" customWidth="1"/>
-    <col min="16" max="16" width="39.33203125" customWidth="1"/>
+    <col min="3" max="3" width="13.36328125" customWidth="1"/>
+    <col min="4" max="4" width="40.453125" customWidth="1"/>
+    <col min="5" max="5" width="13.36328125" customWidth="1"/>
+    <col min="6" max="6" width="39.36328125" customWidth="1"/>
+    <col min="7" max="7" width="13.36328125" customWidth="1"/>
+    <col min="8" max="8" width="39.36328125" customWidth="1"/>
+    <col min="9" max="9" width="13.36328125" customWidth="1"/>
+    <col min="10" max="10" width="39.36328125" customWidth="1"/>
+    <col min="11" max="11" width="13.36328125" customWidth="1"/>
+    <col min="12" max="12" width="39.36328125" customWidth="1"/>
+    <col min="13" max="13" width="13.36328125" customWidth="1"/>
+    <col min="14" max="14" width="39.36328125" customWidth="1"/>
+    <col min="15" max="15" width="13.36328125" customWidth="1"/>
+    <col min="16" max="16" width="39.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:16" ht="19" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:16" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B3" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="2:16" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="5" spans="2:16" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="C5" s="45" t="s">
         <v>37</v>
       </c>
@@ -1649,7 +1649,7 @@
       </c>
       <c r="P5" s="43"/>
     </row>
-    <row r="6" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C6" s="3" t="s">
         <v>4</v>
       </c>
@@ -1693,18 +1693,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="2:16" ht="65" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:16" ht="73" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="7">
-        <v>4.5</v>
-      </c>
-      <c r="D7" s="30" t="s">
-        <v>47</v>
-      </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="8"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="7">
+        <v>8.5</v>
+      </c>
+      <c r="F7" s="30" t="s">
+        <v>48</v>
+      </c>
       <c r="G7" s="9"/>
       <c r="H7" s="10"/>
       <c r="I7" s="9"/>
@@ -1716,15 +1716,17 @@
       <c r="O7" s="9"/>
       <c r="P7" s="10"/>
     </row>
-    <row r="8" spans="2:16" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:16" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="12"/>
       <c r="D8" s="31"/>
-      <c r="E8" s="12"/>
+      <c r="E8" s="12">
+        <v>7.5</v>
+      </c>
       <c r="F8" s="34" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G8" s="14"/>
       <c r="H8" s="37"/>
@@ -1737,7 +1739,7 @@
       <c r="O8" s="14"/>
       <c r="P8" s="37"/>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B9" s="11" t="s">
         <v>10</v>
       </c>
@@ -1756,7 +1758,7 @@
       <c r="O9" s="14"/>
       <c r="P9" s="37"/>
     </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B10" s="11" t="s">
         <v>13</v>
       </c>
@@ -1775,7 +1777,7 @@
       <c r="O10" s="14"/>
       <c r="P10" s="37"/>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B11" s="25" t="s">
         <v>28</v>
       </c>
@@ -1794,7 +1796,7 @@
       <c r="O11" s="28"/>
       <c r="P11" s="38"/>
     </row>
-    <row r="12" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B12" s="16" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
ILV.xlsx meine Stunden eingetragen
</commit_message>
<xml_diff>
--- a/ILV.xlsx
+++ b/ILV.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\i00202920\Documents\GitHub\Pro1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/frank/Pro1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{AC3E5224-F3CB-498F-96DD-ECAEBDD471BD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D537A94A-164C-8F41-B6B2-A9571656CAF1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="22420" windowHeight="14620" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,12 +17,12 @@
     <sheet name="Pflichtenheft org." sheetId="2" r:id="rId2"/>
     <sheet name="Pflichtenheft techn." sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="50">
   <si>
     <t>ILV</t>
   </si>
@@ -199,6 +199,13 @@
 - Kleinere Korrekturen(0.8h) + Batchdatei (0.2h)
 - KIS (1h)
 - Auswertung (4.5h)</t>
+  </si>
+  <si>
+    <t>KIS gegenlesen, verbessern 0.5h
+- Ueberblick.tex 5h
+- Modell.tex 1h
+- Modell.png 0.5h
+- Github diverses. 0.5h</t>
   </si>
 </sst>
 </file>
@@ -796,7 +803,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -880,7 +887,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1182,34 +1189,34 @@
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.453125"/>
-    <col min="2" max="2" width="13.453125"/>
-    <col min="3" max="3" width="12.1796875"/>
-    <col min="4" max="4" width="38.6328125" customWidth="1"/>
-    <col min="5" max="5" width="10.36328125"/>
-    <col min="6" max="6" width="38.6328125" customWidth="1"/>
-    <col min="7" max="7" width="9.453125"/>
-    <col min="8" max="8" width="38.6328125" customWidth="1"/>
-    <col min="9" max="9" width="9.453125"/>
-    <col min="10" max="10" width="28.453125" customWidth="1"/>
-    <col min="11" max="256" width="9.453125"/>
-    <col min="257" max="1025" width="11.453125"/>
+    <col min="1" max="1" width="9.5"/>
+    <col min="2" max="2" width="13.5"/>
+    <col min="3" max="3" width="12.1640625"/>
+    <col min="4" max="4" width="38.6640625" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125"/>
+    <col min="6" max="6" width="38.6640625" customWidth="1"/>
+    <col min="7" max="7" width="9.5"/>
+    <col min="8" max="8" width="38.6640625" customWidth="1"/>
+    <col min="9" max="9" width="9.5"/>
+    <col min="10" max="10" width="28.5" customWidth="1"/>
+    <col min="11" max="256" width="9.5"/>
+    <col min="257" max="1025" width="11.5"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="2:10" ht="24" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:10" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:10" ht="19" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="2:10" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="2:10" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="C7" s="40" t="s">
         <v>2</v>
       </c>
@@ -1227,7 +1234,7 @@
       </c>
       <c r="J7" s="42"/>
     </row>
-    <row r="8" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C8" s="3" t="s">
         <v>4</v>
       </c>
@@ -1253,7 +1260,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="2:10" ht="102" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:10" ht="97" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
         <v>6</v>
       </c>
@@ -1274,7 +1281,7 @@
       <c r="I9" s="9"/>
       <c r="J9" s="10"/>
     </row>
-    <row r="10" spans="2:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:10" ht="48" x14ac:dyDescent="0.2">
       <c r="B10" s="11" t="s">
         <v>9</v>
       </c>
@@ -1295,7 +1302,7 @@
       <c r="I10" s="14"/>
       <c r="J10" s="15"/>
     </row>
-    <row r="11" spans="2:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:10" ht="48" x14ac:dyDescent="0.2">
       <c r="B11" s="11" t="s">
         <v>10</v>
       </c>
@@ -1320,7 +1327,7 @@
       <c r="I11" s="14"/>
       <c r="J11" s="15"/>
     </row>
-    <row r="12" spans="2:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:10" ht="48" x14ac:dyDescent="0.2">
       <c r="B12" s="11" t="s">
         <v>13</v>
       </c>
@@ -1341,7 +1348,7 @@
       <c r="I12" s="14"/>
       <c r="J12" s="15"/>
     </row>
-    <row r="13" spans="2:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:10" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B13" s="16" t="s">
         <v>14</v>
       </c>
@@ -1362,7 +1369,7 @@
       <c r="I13" s="19"/>
       <c r="J13" s="24"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C16" t="s">
         <v>38</v>
       </c>
@@ -1395,32 +1402,32 @@
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.453125"/>
-    <col min="2" max="2" width="13.453125"/>
-    <col min="3" max="3" width="12.1796875"/>
-    <col min="4" max="4" width="39.81640625"/>
-    <col min="5" max="5" width="10.36328125"/>
-    <col min="6" max="6" width="40.453125" customWidth="1"/>
-    <col min="7" max="7" width="9.453125"/>
-    <col min="8" max="8" width="39.81640625"/>
-    <col min="9" max="254" width="9.453125"/>
-    <col min="255" max="1023" width="11.453125"/>
+    <col min="1" max="1" width="9.5"/>
+    <col min="2" max="2" width="13.5"/>
+    <col min="3" max="3" width="12.1640625"/>
+    <col min="4" max="4" width="39.83203125"/>
+    <col min="5" max="5" width="10.33203125"/>
+    <col min="6" max="6" width="40.5" customWidth="1"/>
+    <col min="7" max="7" width="9.5"/>
+    <col min="8" max="8" width="39.83203125"/>
+    <col min="9" max="254" width="9.5"/>
+    <col min="255" max="1023" width="11.5"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="2:8" ht="24" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:8" ht="19" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="2:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:8" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="2:8" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="C7" s="40" t="s">
         <v>15</v>
       </c>
@@ -1434,7 +1441,7 @@
       </c>
       <c r="H7" s="42"/>
     </row>
-    <row r="8" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C8" s="3" t="s">
         <v>4</v>
       </c>
@@ -1454,7 +1461,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="58.5" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:8" ht="49" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
         <v>6</v>
       </c>
@@ -1473,7 +1480,7 @@
       <c r="G9" s="9"/>
       <c r="H9" s="22"/>
     </row>
-    <row r="10" spans="2:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:8" ht="32" x14ac:dyDescent="0.2">
       <c r="B10" s="11" t="s">
         <v>9</v>
       </c>
@@ -1496,7 +1503,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="2:8" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:8" ht="64" x14ac:dyDescent="0.2">
       <c r="B11" s="11" t="s">
         <v>10</v>
       </c>
@@ -1519,7 +1526,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="2:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:8" ht="32" x14ac:dyDescent="0.2">
       <c r="B12" s="11" t="s">
         <v>13</v>
       </c>
@@ -1538,7 +1545,7 @@
       <c r="G12" s="14"/>
       <c r="H12" s="15"/>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B13" s="25" t="s">
         <v>28</v>
       </c>
@@ -1553,7 +1560,7 @@
       <c r="G13" s="28"/>
       <c r="H13" s="29"/>
     </row>
-    <row r="14" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B14" s="16" t="s">
         <v>14</v>
       </c>
@@ -1592,34 +1599,34 @@
   <dimension ref="B3:P12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="13.36328125" customWidth="1"/>
-    <col min="4" max="4" width="40.453125" customWidth="1"/>
-    <col min="5" max="5" width="13.36328125" customWidth="1"/>
-    <col min="6" max="6" width="39.36328125" customWidth="1"/>
-    <col min="7" max="7" width="13.36328125" customWidth="1"/>
-    <col min="8" max="8" width="39.36328125" customWidth="1"/>
-    <col min="9" max="9" width="13.36328125" customWidth="1"/>
-    <col min="10" max="10" width="39.36328125" customWidth="1"/>
-    <col min="11" max="11" width="13.36328125" customWidth="1"/>
-    <col min="12" max="12" width="39.36328125" customWidth="1"/>
-    <col min="13" max="13" width="13.36328125" customWidth="1"/>
-    <col min="14" max="14" width="39.36328125" customWidth="1"/>
-    <col min="15" max="15" width="13.36328125" customWidth="1"/>
-    <col min="16" max="16" width="39.36328125" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" customWidth="1"/>
+    <col min="4" max="4" width="40.5" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" customWidth="1"/>
+    <col min="6" max="6" width="39.33203125" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" customWidth="1"/>
+    <col min="8" max="8" width="39.33203125" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" customWidth="1"/>
+    <col min="10" max="10" width="39.33203125" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" customWidth="1"/>
+    <col min="12" max="12" width="39.33203125" customWidth="1"/>
+    <col min="13" max="13" width="13.33203125" customWidth="1"/>
+    <col min="14" max="14" width="39.33203125" customWidth="1"/>
+    <col min="15" max="15" width="13.33203125" customWidth="1"/>
+    <col min="16" max="16" width="39.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:16" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:16" ht="19" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="5" spans="2:16" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="2:16" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="C5" s="45" t="s">
         <v>37</v>
       </c>
@@ -1649,7 +1656,7 @@
       </c>
       <c r="P5" s="43"/>
     </row>
-    <row r="6" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C6" s="3" t="s">
         <v>4</v>
       </c>
@@ -1693,7 +1700,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="2:16" ht="73" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:16" ht="65" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B7" s="6" t="s">
         <v>6</v>
       </c>
@@ -1716,7 +1723,7 @@
       <c r="O7" s="9"/>
       <c r="P7" s="10"/>
     </row>
-    <row r="8" spans="2:16" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:16" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="11" t="s">
         <v>9</v>
       </c>
@@ -1739,14 +1746,18 @@
       <c r="O8" s="14"/>
       <c r="P8" s="37"/>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:16" ht="80" x14ac:dyDescent="0.2">
       <c r="B9" s="11" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="12"/>
       <c r="D9" s="31"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="34"/>
+      <c r="E9" s="12">
+        <v>7.5</v>
+      </c>
+      <c r="F9" s="34" t="s">
+        <v>49</v>
+      </c>
       <c r="G9" s="14"/>
       <c r="H9" s="37"/>
       <c r="I9" s="14"/>
@@ -1758,7 +1769,7 @@
       <c r="O9" s="14"/>
       <c r="P9" s="37"/>
     </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B10" s="11" t="s">
         <v>13</v>
       </c>
@@ -1777,7 +1788,7 @@
       <c r="O10" s="14"/>
       <c r="P10" s="37"/>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B11" s="25" t="s">
         <v>28</v>
       </c>
@@ -1796,7 +1807,7 @@
       <c r="O11" s="28"/>
       <c r="P11" s="38"/>
     </row>
-    <row r="12" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="16" t="s">
         <v>14</v>
       </c>

</xml_diff>